<commit_message>
Fixed spelling of Vadegræssamfund
</commit_message>
<xml_diff>
--- a/data-raw/Habitat_types_DFV_v2.xlsx
+++ b/data-raw/Habitat_types_DFV_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aarhus_Uni\DanskFloraVegetation\Pensum\Naturtyper_pensum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au650181_uni_au_dk/Documents/generel/github/FloraExam/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E2FFF7-5B14-4852-A556-9CB2A6C31792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{70E2FFF7-5B14-4852-A556-9CB2A6C31792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3450D3F1-01D3-4EC1-8A4B-6A2D07FA763C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>Strandvold med flerårige planter</t>
   </si>
   <si>
-    <t>Vædegrassamfund</t>
-  </si>
-  <si>
     <t>Enårig strandengsvegetation</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>Elle- og askeskov</t>
+  </si>
+  <si>
+    <t>Vadegræssamfund</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,13 +631,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -673,13 +673,13 @@
         <v>1310</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -687,13 +687,13 @@
         <v>1320</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,13 +743,13 @@
         <v>2130</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,13 +813,13 @@
         <v>6120</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5">
         <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +861,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,13 +869,13 @@
         <v>7110</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -917,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -959,7 +959,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1001,7 +1001,7 @@
         <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1009,13 +1009,13 @@
         <v>9160</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>22</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1043,7 +1043,7 @@
         <v>22</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
         <v>22</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="3">
         <v>9998</v>
@@ -1068,13 +1068,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E32" s="3">
         <v>9999</v>
@@ -1104,60 +1104,60 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="7"/>
     </row>

</xml_diff>